<commit_message>
nearly done but damn
</commit_message>
<xml_diff>
--- a/modeling/logistic.xlsx
+++ b/modeling/logistic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Quynh\Routing_optimization\modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24D23208-C74C-4E0A-96A3-939682A4BF1B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42C2DBFB-2404-4120-86F7-659189AD6B1E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="570" yWindow="1335" windowWidth="21600" windowHeight="12915" activeTab="3" xr2:uid="{298FD6C0-0A5D-4939-95FB-5AA249284DA3}"/>
+    <workbookView xWindow="14520" yWindow="3540" windowWidth="21600" windowHeight="9915" activeTab="3" xr2:uid="{298FD6C0-0A5D-4939-95FB-5AA249284DA3}"/>
   </bookViews>
   <sheets>
     <sheet name="ROUTE OPTIMIZATION " sheetId="9" r:id="rId1"/>
@@ -238,11 +238,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -567,132 +567,126 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="10"/>
+      <c r="D2" s="10"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="J3" s="10" t="s">
+      <c r="B3" s="10"/>
+      <c r="C3" s="10"/>
+      <c r="D3" s="10"/>
+      <c r="E3" s="10"/>
+      <c r="F3" s="10"/>
+      <c r="G3" s="10"/>
+      <c r="J3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="10" t="s">
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="10"/>
-      <c r="P3" s="10"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="J4" s="10" t="s">
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="10"/>
+      <c r="J4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10" t="s">
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="J5" s="10" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="10"/>
+      <c r="J5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-      <c r="N5" s="10" t="s">
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="10"/>
-      <c r="P5" s="10"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="J6" s="10" t="s">
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="10"/>
+      <c r="J6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10" t="s">
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="10"/>
-      <c r="P6" s="10"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="10"/>
+      <c r="D8" s="10"/>
+      <c r="E8" s="10"/>
+      <c r="F8" s="10"/>
+      <c r="G8" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A4:G5"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:G7"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="J5:M5"/>
@@ -701,6 +695,12 @@
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="N5:P5"/>
     <mergeCell ref="N6:P6"/>
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A4:G5"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -712,7 +712,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1126,7 +1126,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1524,7 +1524,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,7 +1572,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>20</v>
@@ -1583,7 +1583,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>10</v>
+        <v>4.5</v>
       </c>
       <c r="C5" s="1">
         <v>17</v>
@@ -1616,10 +1616,10 @@
         <v>6</v>
       </c>
       <c r="B8" s="1">
-        <v>11</v>
+        <v>3.5</v>
       </c>
       <c r="C8" s="1">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
fix constraint time 2 3
</commit_message>
<xml_diff>
--- a/modeling/logistic.xlsx
+++ b/modeling/logistic.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Quynh\Routing_optimization\modeling\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nguye\Downloads\Routing_optimization\modeling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2937E016-CAE1-48BF-8671-959E636D00A0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7DFCE47-65F4-40D9-8D2C-C146A57F4FE3}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16650" yWindow="2235" windowWidth="14235" windowHeight="9915" firstSheet="1" activeTab="1" xr2:uid="{298FD6C0-0A5D-4939-95FB-5AA249284DA3}"/>
+    <workbookView xWindow="10215" yWindow="1410" windowWidth="15015" windowHeight="7860" firstSheet="3" activeTab="5" xr2:uid="{298FD6C0-0A5D-4939-95FB-5AA249284DA3}"/>
   </bookViews>
   <sheets>
     <sheet name="ROUTE OPTIMIZATION " sheetId="9" r:id="rId1"/>
@@ -245,11 +245,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -574,126 +574,132 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="2" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="11" t="s">
+      <c r="A2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="11"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="11"/>
-      <c r="F2" s="11"/>
-      <c r="G2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="11"/>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
-      <c r="F3" s="11"/>
-      <c r="G3" s="11"/>
-      <c r="J3" s="12" t="s">
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="J3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="K3" s="12"/>
-      <c r="L3" s="12"/>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12" t="s">
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="O3" s="12"/>
-      <c r="P3" s="12"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
     </row>
     <row r="4" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
+      <c r="A4" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
-      <c r="F4" s="11"/>
-      <c r="G4" s="11"/>
-      <c r="J4" s="12" t="s">
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="J4" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="K4" s="12"/>
-      <c r="L4" s="12"/>
-      <c r="M4" s="12"/>
-      <c r="N4" s="12" t="s">
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="O4" s="12"/>
-      <c r="P4" s="12"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
     </row>
     <row r="5" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="J5" s="12" t="s">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="J5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="12" t="s">
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="O5" s="12"/>
-      <c r="P5" s="12"/>
+      <c r="O5" s="11"/>
+      <c r="P5" s="11"/>
     </row>
     <row r="6" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
+      <c r="A6" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
-      <c r="F6" s="11"/>
-      <c r="G6" s="11"/>
-      <c r="J6" s="12" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
+      <c r="G6" s="12"/>
+      <c r="J6" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="12"/>
-      <c r="L6" s="12"/>
-      <c r="M6" s="12"/>
-      <c r="N6" s="12" t="s">
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="O6" s="12"/>
-      <c r="P6" s="12"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="11" t="s">
+      <c r="A7" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
+      <c r="A8" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A8:G8"/>
+    <mergeCell ref="A4:G5"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+    <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A7:G7"/>
     <mergeCell ref="J3:M3"/>
     <mergeCell ref="J4:M4"/>
     <mergeCell ref="J5:M5"/>
@@ -702,12 +708,6 @@
     <mergeCell ref="N4:P4"/>
     <mergeCell ref="N5:P5"/>
     <mergeCell ref="N6:P6"/>
-    <mergeCell ref="A8:G8"/>
-    <mergeCell ref="A4:G5"/>
-    <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A3:G3"/>
-    <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A7:G7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -718,8 +718,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EADC77A-A9A0-442C-9D68-575FC0198A66}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -779,7 +779,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D2" s="6">
         <v>4.5</v>
@@ -811,7 +811,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="6">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="C3" s="6">
         <v>0</v>
@@ -1560,7 +1560,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1568,7 +1568,7 @@
         <v>1</v>
       </c>
       <c r="B3" s="1">
-        <v>7</v>
+        <v>10</v>
       </c>
       <c r="C3" s="1">
         <v>13</v>
@@ -1579,10 +1579,10 @@
         <v>2</v>
       </c>
       <c r="B4" s="1">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1590,7 +1590,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1">
-        <v>3.5</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>17</v>
@@ -1612,7 +1612,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="1">
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="C7" s="1">
         <v>15</v>
@@ -1626,7 +1626,7 @@
         <v>0</v>
       </c>
       <c r="C8" s="1">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1645,10 +1645,10 @@
         <v>8</v>
       </c>
       <c r="B10" s="1">
-        <v>4.5</v>
+        <v>11</v>
       </c>
       <c r="C10" s="1">
-        <v>10.5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1659,7 +1659,7 @@
         <v>6</v>
       </c>
       <c r="C11" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1672,7 +1672,7 @@
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N12" sqref="N12:N13"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1688,7 +1688,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1696,7 +1696,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1">
-        <v>45</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1720,7 +1720,7 @@
         <v>6</v>
       </c>
       <c r="B6" s="1">
-        <v>22</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1728,7 +1728,7 @@
         <v>7</v>
       </c>
       <c r="B7" s="1">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C697A500-E27F-4E63-9779-90EBED01BD57}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -1785,7 +1785,7 @@
         <v>13</v>
       </c>
       <c r="B2" s="1">
-        <v>100</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1793,7 +1793,7 @@
         <v>14</v>
       </c>
       <c r="B3" s="1">
-        <v>70</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -1801,7 +1801,7 @@
         <v>15</v>
       </c>
       <c r="B4" s="1">
-        <v>145</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -1809,7 +1809,7 @@
         <v>16</v>
       </c>
       <c r="B5" s="1">
-        <v>90</v>
+        <v>150</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -1832,7 +1832,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>